<commit_message>
reimplement the multiplier for 30KV P-P tradeoffs
</commit_message>
<xml_diff>
--- a/EHD/Multiplier-working-12x20.xlsx
+++ b/EHD/Multiplier-working-12x20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/projects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/MolecularKinetics/EHD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E28506-6D46-9F41-807D-26D8145ED429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CF74B8-3F7E-4A47-B55A-A1AA8426B8EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1320" yWindow="500" windowWidth="26580" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:T5688"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1491,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="12">
-        <v>100000</v>
+        <v>120000</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>31</v>
@@ -1524,7 +1524,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="13">
-        <v>1E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>30</v>
@@ -1546,7 +1546,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="14">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>32</v>
@@ -1586,7 +1586,7 @@
       <c r="D13" s="10"/>
       <c r="F13" s="24">
         <f>C10/F12</f>
-        <v>2.5000000000000001E-5</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>47</v>
@@ -1607,7 +1607,7 @@
     <row r="14" spans="1:13" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="F14" s="25">
         <f>C10*F13</f>
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>48</v>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="F15" s="26">
         <f>C10*C11</f>
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>49</v>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="C17" s="41">
         <f>+C10*C15/100</f>
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="D17" s="39" t="s">
         <v>35</v>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="C18" s="42">
         <f>+C11*(C12*C12+C12/2)/8/C13/C17</f>
-        <v>1.8749999999999998E-9</v>
+        <v>1.640625E-9</v>
       </c>
       <c r="D18" s="39" t="s">
         <v>53</v>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="C19" s="43">
         <f>+(C10+(C10*C16/100))*2/C12</f>
-        <v>17500</v>
+        <v>25200</v>
       </c>
       <c r="D19" s="39" t="s">
         <v>36</v>
@@ -1772,7 +1772,7 @@
       </c>
       <c r="C20" s="43">
         <f>+C10*C16/(100)</f>
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="D20" s="39" t="s">
         <v>37</v>
@@ -1817,14 +1817,14 @@
       </c>
       <c r="C21" s="44">
         <f>+C$11*(C$12*C$12*C$12+C$12*C$12*9/4+C$12/2)/12/C$13/C$20</f>
-        <v>1.715E-9</v>
+        <v>1.2812500000000001E-9</v>
       </c>
       <c r="D21" s="39" t="s">
         <v>52</v>
       </c>
       <c r="F21" s="31">
         <f>C28</f>
-        <v>17535.460992907803</v>
+        <v>24512.5</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>58</v>
@@ -1914,15 +1914,15 @@
         <v>23</v>
       </c>
       <c r="C23" s="13">
-        <f>0.0000000047 * 0.35</f>
-        <v>1.6449999999999998E-9</v>
+        <f>0.000000003</f>
+        <v>3E-9</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F23" s="32">
         <f>F21/F19</f>
-        <v>561.13475177304974</v>
+        <v>784.4</v>
       </c>
       <c r="G23" s="23" t="s">
         <v>55</v>
@@ -1967,14 +1967,14 @@
       </c>
       <c r="C24" s="17">
         <f>+(+C12*C12+C12/2)*C11/8/C13/C23/C10</f>
-        <v>5.6990881458966565E-3</v>
+        <v>2.7343749999999998E-3</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="32">
         <f>F23/2</f>
-        <v>280.56737588652487</v>
+        <v>392.2</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>59</v>
@@ -2024,14 +2024,14 @@
       </c>
       <c r="C25" s="17">
         <f>+C$11*(C$12*C$12*C$12+C$12*C$12*9/4+C$12/2)/12/C$13/C$23/C$10</f>
-        <v>5.2127659574468091E-2</v>
+        <v>2.1354166666666667E-2</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>40</v>
       </c>
       <c r="F25" s="35">
         <f>F24/1.414</f>
-        <v>198.4210579112623</v>
+        <v>277.3691654879774</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>63</v>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="C26" s="28">
         <f>+(+C12*C12+C12/2)*C11/8/C13/C23</f>
-        <v>569.90881458966567</v>
+        <v>328.125</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>51</v>
@@ -2133,14 +2133,14 @@
       </c>
       <c r="C27" s="18">
         <f>+C$11*(C$12*C$12*C$12+C$12*C$12*9/4+C$12/2)/12/C$13/C$23</f>
-        <v>5212.7659574468089</v>
+        <v>2562.5</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>54</v>
       </c>
       <c r="F27" s="33">
         <f>F15/F21*2</f>
-        <v>1.140546006066734E-2</v>
+        <v>1.4686384497705252E-2</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>138</v>
@@ -2155,14 +2155,14 @@
       </c>
       <c r="C28" s="16">
         <f>(+C10+C27)/C12*2</f>
-        <v>17535.460992907803</v>
+        <v>24512.5</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>73</v>
       </c>
       <c r="F28" s="34">
         <f>F27*(F18/F17)</f>
-        <v>0.35642062689585435</v>
+        <v>0.45894951555328911</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>139</v>
@@ -2202,7 +2202,7 @@
       <c r="B29" s="4"/>
       <c r="C29" s="65">
         <f>C28/2</f>
-        <v>8767.7304964539017</v>
+        <v>12256.25</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>148</v>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="F60" s="62">
         <f>F28/2</f>
-        <v>0.17821031344792718</v>
+        <v>0.22947475777664456</v>
       </c>
       <c r="G60" s="54" t="s">
         <v>140</v>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F61" s="56">
         <f>F60/(4*120*(F59/1000000))</f>
-        <v>0.7425429726996966</v>
+        <v>0.95614482406935231</v>
       </c>
       <c r="G61" s="54" t="s">
         <v>136</v>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="F62" s="56">
         <f>F60/(120*(F59/1000000))</f>
-        <v>2.9701718907987864</v>
+        <v>3.8245792962774092</v>
       </c>
       <c r="G62" s="54" t="s">
         <v>137</v>

</xml_diff>